<commit_message>
In class WBT tests(lab 3)
</commit_message>
<xml_diff>
--- a/EC_BVA.xlsx
+++ b/EC_BVA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>EC</t>
   </si>
@@ -89,12 +89,6 @@
     <t>grupa in [110…938]</t>
   </si>
   <si>
-    <t>grupa &lt;110</t>
-  </si>
-  <si>
-    <t>grupa &gt;938</t>
-  </si>
-  <si>
     <t>BVA</t>
   </si>
   <si>
@@ -105,6 +99,15 @@
   </si>
   <si>
     <t>maxInt +1</t>
+  </si>
+  <si>
+    <t>grupa in [111…938]</t>
+  </si>
+  <si>
+    <t>grupa &lt;111</t>
+  </si>
+  <si>
+    <t>grupa &gt;937</t>
   </si>
 </sst>
 </file>
@@ -440,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -563,7 +566,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -579,7 +582,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -590,12 +593,12 @@
         <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -605,7 +608,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
@@ -613,11 +616,13 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>18</v>
@@ -629,37 +634,37 @@
         <v>20</v>
       </c>
       <c r="H17" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G18" s="1"/>
       <c r="H18" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>
       <c r="H19" s="1">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G20" s="1"/>
       <c r="H20" s="1">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
       <c r="H21" s="1">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
       <c r="H22" s="1">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>